<commit_message>
Write excel datas add
</commit_message>
<xml_diff>
--- a/src/resources/takimlar.xlsx
+++ b/src/resources/takimlar.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alitu\IdeaProjects\JUnitFramework\src\resources\"/>
     </mc:Choice>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="49">
   <si>
     <t xml:space="preserve">Ülke </t>
   </si>
@@ -170,12 +170,16 @@
   </si>
   <si>
     <t>yeni Olusturuldu</t>
+  </si>
+  <si>
+    <t>Puan</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="0"/>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -472,7 +476,7 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="26" width="28.7109375" customWidth="1"/>
+    <col min="1" max="26" customWidth="true" width="28.7109375"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -488,8 +492,8 @@
       <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" t="s">
-        <v>44</v>
+      <c r="E1" t="s" s="0">
+        <v>48</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -505,8 +509,8 @@
       <c r="D2" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="E2" t="s">
-        <v>45</v>
+      <c r="E2" t="n" s="0">
+        <v>85.0</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -516,7 +520,7 @@
       <c r="B3" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" t="s" s="0">
         <v>9</v>
       </c>
       <c r="D3" s="2" t="s">
@@ -550,8 +554,8 @@
       <c r="D5" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="E5" t="s">
-        <v>47</v>
+      <c r="E5" t="n" s="0">
+        <v>78.0</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
@@ -623,8 +627,8 @@
       <c r="D10" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="E10" t="s">
-        <v>46</v>
+      <c r="E10" t="n" s="0">
+        <v>72.0</v>
       </c>
     </row>
     <row r="21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Delete excel datas remove
</commit_message>
<xml_diff>
--- a/src/resources/takimlar.xlsx
+++ b/src/resources/takimlar.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alitu\IdeaProjects\JUnitFramework\src\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6DCD3062-9DAA-4C56-BE6E-7736447AC34C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{745F0FE0-DDDB-4C08-BDE9-4AC281358BCF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3420" yWindow="3420" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sayfa1" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="45">
   <si>
     <t xml:space="preserve">Ülke </t>
   </si>
@@ -158,18 +158,6 @@
   </si>
   <si>
     <t>qwerty</t>
-  </si>
-  <si>
-    <t>PUAN</t>
-  </si>
-  <si>
-    <t>85</t>
-  </si>
-  <si>
-    <t>72</t>
-  </si>
-  <si>
-    <t>yeni Olusturuldu</t>
   </si>
   <si>
     <t>Puan</t>
@@ -471,7 +459,7 @@
   <dimension ref="A1:E1000"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -493,7 +481,7 @@
         <v>2</v>
       </c>
       <c r="E1" t="s" s="0">
-        <v>48</v>
+        <v>44</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -509,8 +497,8 @@
       <c r="D2" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="E2" t="n" s="0">
-        <v>85.0</v>
+      <c r="E2" s="0">
+        <v>85</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -520,9 +508,6 @@
       <c r="B3" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C3" t="s" s="0">
-        <v>9</v>
-      </c>
       <c r="D3" s="2" t="s">
         <v>10</v>
       </c>
@@ -554,8 +539,8 @@
       <c r="D5" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="E5" t="n" s="0">
-        <v>78.0</v>
+      <c r="E5" s="0">
+        <v>78</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
@@ -627,8 +612,8 @@
       <c r="D10" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="E10" t="n" s="0">
-        <v>72.0</v>
+      <c r="E10" s="0">
+        <v>72</v>
       </c>
     </row>
     <row r="21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>